<commit_message>
Já está pegando todos os grupos, excetos os verdadeiros sozinhos e faltar gerar a string
</commit_message>
<xml_diff>
--- a/Map.xlsx
+++ b/Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adrya\OneDrive\Área de Trabalho\Programação\Projetos pessoais\Karnaugh-Map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE8EBB4-E71D-49D9-BD54-3BC3D2C39BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E91ABE-9903-4108-ADDB-99B004698034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>A</t>
   </si>
@@ -51,19 +51,34 @@
     <t>S</t>
   </si>
   <si>
-    <t>A - B/C</t>
-  </si>
-  <si>
-    <t>"00"</t>
-  </si>
-  <si>
-    <t>"01"</t>
-  </si>
-  <si>
-    <t>"11"</t>
-  </si>
-  <si>
-    <t>"10"</t>
+    <t>V</t>
+  </si>
+  <si>
+    <t>"-D-A"</t>
+  </si>
+  <si>
+    <t>"-DA"</t>
+  </si>
+  <si>
+    <t>"DA"</t>
+  </si>
+  <si>
+    <t>"D-A"</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>"-BC"</t>
+  </si>
+  <si>
+    <t>"-B-C"</t>
+  </si>
+  <si>
+    <t>"BC"</t>
+  </si>
+  <si>
+    <t>"B-C"</t>
   </si>
 </sst>
 </file>
@@ -114,13 +129,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -403,13 +421,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -422,6 +443,9 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="3"/>
@@ -437,6 +461,9 @@
         <v>0</v>
       </c>
       <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
         <v>1</v>
       </c>
     </row>
@@ -451,6 +478,9 @@
         <v>1</v>
       </c>
       <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
         <v>1</v>
       </c>
     </row>
@@ -467,6 +497,9 @@
       <c r="D4" s="2">
         <v>0</v>
       </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -481,6 +514,9 @@
       <c r="D5" s="2">
         <v>0</v>
       </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -495,6 +531,9 @@
       <c r="D6" s="2">
         <v>0</v>
       </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -509,6 +548,9 @@
       <c r="D7" s="2">
         <v>0</v>
       </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -523,6 +565,9 @@
       <c r="D8" s="2">
         <v>0</v>
       </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -535,6 +580,145 @@
         <v>1</v>
       </c>
       <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>0</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>0</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>1</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>1</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2">
         <v>0</v>
       </c>
     </row>
@@ -545,10 +729,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69E5E80-7680-4232-B8C3-1D2D7A4D1F30}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,57 +742,99 @@
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="1">
+        <f>(Plan1!E2)</f>
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <f>(Plan1!E3)</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <f>(Plan1!E5)</f>
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <f>(Plan1!E4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B3" s="1">
+        <f>(Plan1!E6)</f>
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <f>(Plan1!E7)</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <f>(Plan1!E9)</f>
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <f>(Plan1!E8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B4" s="1">
+        <f>(Plan1!E14)</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <f>(Plan1!E15)</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <f>(Plan1!E17)</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <f>(Plan1!E16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1">
-        <f>(Plan1!D2)</f>
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <f>(Plan1!D3)</f>
-        <v>1</v>
-      </c>
-      <c r="D2" s="1">
-        <f>(Plan1!D5)</f>
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
-        <f>(Plan1!D4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <f>(Plan1!D6)</f>
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <f>(Plan1!D7)</f>
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
-        <f>(Plan1!D9)</f>
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <f>(Plan1!D8)</f>
+      <c r="B5" s="1">
+        <f>(Plan1!E10)</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <f>(Plan1!E11)</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <f>(Plan1!E13)</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <f>(Plan1!E12)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finalizado o de 4 e 3 variáveis
</commit_message>
<xml_diff>
--- a/Map.xlsx
+++ b/Map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adrya\OneDrive\Área de Trabalho\Programação\Projetos pessoais\Karnaugh-Map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E91ABE-9903-4108-ADDB-99B004698034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58B16D5-0F0E-4D3B-AF7C-432EB71817F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2895" yWindow="2895" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -423,8 +423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,7 +464,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -481,7 +481,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -498,7 +498,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -515,7 +515,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -583,7 +583,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -668,7 +668,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -685,7 +685,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -732,7 +732,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,19 +760,19 @@
       </c>
       <c r="B2" s="1">
         <f>(Plan1!E2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1">
         <f>(Plan1!E3)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="1">
         <f>(Plan1!E5)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="1">
         <f>(Plan1!E4)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -789,7 +789,7 @@
       </c>
       <c r="D3" s="1">
         <f>(Plan1!E9)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1">
         <f>(Plan1!E8)</f>
@@ -802,11 +802,11 @@
       </c>
       <c r="B4" s="1">
         <f>(Plan1!E14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1">
         <f>(Plan1!E15)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="1">
         <f>(Plan1!E17)</f>

</xml_diff>